<commit_message>
New data for English version of dashboard
</commit_message>
<xml_diff>
--- a/data/en/outcome_table.xlsx
+++ b/data/en/outcome_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidpietersz/Library/CloudStorage/OneDrive-ErasmusUniversityRotterdam/Kansenlab/kenniscentrumongelijkheid-main/data/en/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidpietersz/Documents/GitHub/kenniscentrumongelijkheid/data/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0446FB07-7C28-524E-B979-A9EDF07D8353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E5D860-987B-A548-8ECF-F6A8955CD222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
     <t>refers to average annual total care costs, covered by the Health Insurance Act, of 16-year-olds in the year that they turned 16.</t>
   </si>
   <si>
-    <t>c21_young_parent</t>
+    <t>c21_young_parents</t>
   </si>
   <si>
     <t>Young Parenthood</t>
@@ -144,15 +144,18 @@
     <t>refers to the percentage of 21-year-old parents who became a parent before they turned 20</t>
   </si>
   <si>
+    <t>21-Year-Olds</t>
+  </si>
+  <si>
+    <t>c30_total_health_costs</t>
+  </si>
+  <si>
+    <t>refers to average total health care costs covered by the Health Insurance Act, of 35-year-olds in the year that they turned 35.</t>
+  </si>
+  <si>
     <t>35-Year-Olds</t>
   </si>
   <si>
-    <t>c30_total_health_costs</t>
-  </si>
-  <si>
-    <t>refers to average total health care costs covered by the Health Insurance Act, of 35-year-olds in the year that they turned 35.</t>
-  </si>
-  <si>
     <t>c30_hospital</t>
   </si>
   <si>
@@ -327,9 +330,6 @@
     <t>refers to the percentage of 21-year-olds with a high school degree (havo, vwo, or mbo level 2 of higher).</t>
   </si>
   <si>
-    <t>21-Year-Olds</t>
-  </si>
-  <si>
     <t>c21_hbo_followed</t>
   </si>
   <si>
@@ -546,7 +546,7 @@
     <t>years</t>
   </si>
   <si>
-    <t>c35_age_left_parents</t>
+    <t>c30_age_left_parents</t>
   </si>
   <si>
     <t>Age left parental home</t>
@@ -561,7 +561,7 @@
     <t>refers to the average home size per household member of 35-year-olds.</t>
   </si>
   <si>
-    <t>c30_home_owner</t>
+    <t>c30_homeowner</t>
   </si>
   <si>
     <t>Home Owner</t>
@@ -819,7 +819,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -838,6 +838,12 @@
         <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -851,7 +857,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -878,6 +884,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="128.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,7 +1460,7 @@
         <v>33</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -1473,7 +1480,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1481,19 +1488,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1501,19 +1508,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1521,19 +1528,19 @@
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1541,19 +1548,19 @@
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1561,16 +1568,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>21</v>
@@ -1581,16 +1588,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>21</v>
@@ -1601,16 +1608,16 @@
         <v>6</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>21</v>
@@ -1621,16 +1628,16 @@
         <v>6</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>21</v>
@@ -1641,16 +1648,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>21</v>
@@ -1661,16 +1668,16 @@
         <v>6</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>21</v>
@@ -1681,16 +1688,16 @@
         <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>21</v>
@@ -1701,16 +1708,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>21</v>
@@ -1721,16 +1728,16 @@
         <v>6</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>21</v>
@@ -1741,16 +1748,16 @@
         <v>6</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>21</v>
@@ -1761,16 +1768,16 @@
         <v>6</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>21</v>
@@ -1781,16 +1788,16 @@
         <v>6</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>28</v>
@@ -1801,16 +1808,16 @@
         <v>6</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>28</v>
@@ -1821,16 +1828,16 @@
         <v>6</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>28</v>
@@ -1841,19 +1848,19 @@
         <v>6</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1867,13 +1874,13 @@
         <v>97</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1887,13 +1894,13 @@
         <v>100</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -1907,13 +1914,13 @@
         <v>103</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>104</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1927,390 +1934,390 @@
         <v>106</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>118</v>
+      <c r="A34" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>159</v>
+        <v>112</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>28</v>
+        <v>110</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>165</v>
+      <c r="B36" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>166</v>
+        <v>110</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>169</v>
+        <v>118</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>170</v>
+        <v>110</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>159</v>
+        <v>6</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>172</v>
+        <v>110</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>174</v>
+        <v>22</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>175</v>
+        <v>110</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>22</v>
+      <c r="A40" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>109</v>
+        <v>128</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>111</v>
+      <c r="E40" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>113</v>
+        <v>131</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>116</v>
+      <c r="B42" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>119</v>
+        <v>6</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>110</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>123</v>
+        <v>22</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>124</v>
+      <c r="E44" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>125</v>
+      <c r="B45" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>127</v>
+      <c r="E45" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>129</v>
+        <v>146</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>130</v>
+      <c r="E46" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>132</v>
+        <v>149</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E47" s="9" t="s">
-        <v>133</v>
+      <c r="E47" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>135</v>
+        <v>152</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>136</v>
+      <c r="E48" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>138</v>
+        <v>155</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>156</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>139</v>
+      <c r="E49" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>110</v>
+        <v>158</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>160</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>110</v>
+        <v>162</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>160</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>34</v>
+        <v>163</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>148</v>
+        <v>165</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>166</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>34</v>
@@ -2318,62 +2325,62 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>151</v>
+        <v>169</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>110</v>
+        <v>171</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>160</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>157</v>
+        <v>173</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
delete dissolved municipalities from options
</commit_message>
<xml_diff>
--- a/data/en/outcome_table.xlsx
+++ b/data/en/outcome_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidpietersz/Documents/GitHub/kenniscentrumongelijkheid/data/en/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilsonea/Documents/GitHub/kenniscentrumongelijkheid/data/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E5D860-987B-A548-8ECF-F6A8955CD222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8286BD-7579-5042-9E93-16A5F948304A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="243">
   <si>
     <t>prefix_postfix</t>
   </si>
@@ -751,9 +749,6 @@
   </si>
   <si>
     <t>Ouder-Amstel</t>
-  </si>
-  <si>
-    <t>Beemster</t>
   </si>
   <si>
     <t>Landsmeer</t>
@@ -971,9 +966,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1011,7 +1006,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1117,7 +1112,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1259,7 +1254,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1269,7 +1264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2401,10 +2396,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2898,7 +2893,7 @@
         <v>241</v>
       </c>
       <c r="B61" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2906,14 +2901,6 @@
         <v>242</v>
       </c>
       <c r="B62" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>243</v>
-      </c>
-      <c r="B63" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
delete dissolved municipalities from options (#100)
</commit_message>
<xml_diff>
--- a/data/en/outcome_table.xlsx
+++ b/data/en/outcome_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidpietersz/Documents/GitHub/kenniscentrumongelijkheid/data/en/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilsonea/Documents/GitHub/kenniscentrumongelijkheid/data/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E5D860-987B-A548-8ECF-F6A8955CD222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8286BD-7579-5042-9E93-16A5F948304A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="243">
   <si>
     <t>prefix_postfix</t>
   </si>
@@ -751,9 +749,6 @@
   </si>
   <si>
     <t>Ouder-Amstel</t>
-  </si>
-  <si>
-    <t>Beemster</t>
   </si>
   <si>
     <t>Landsmeer</t>
@@ -971,9 +966,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1011,7 +1006,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1117,7 +1112,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1259,7 +1254,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1269,7 +1264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2401,10 +2396,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2898,7 +2893,7 @@
         <v>241</v>
       </c>
       <c r="B61" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2906,14 +2901,6 @@
         <v>242</v>
       </c>
       <c r="B62" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>243</v>
-      </c>
-      <c r="B63" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>